<commit_message>
header separado + EL EXCEL FUNCIONA
</commit_message>
<xml_diff>
--- a/upload-excel/excel_value.xlsx
+++ b/upload-excel/excel_value.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>legajo_profesor</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>minuto_fin</t>
+  </si>
+  <si>
+    <t>B101</t>
+  </si>
+  <si>
+    <t>S354</t>
+  </si>
+  <si>
+    <t>S489</t>
   </si>
 </sst>
 </file>
@@ -385,7 +394,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,10 +431,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1123</v>
-      </c>
-      <c r="B2">
-        <v>500</v>
+        <v>105698</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="2">
         <v>12</v>
@@ -445,10 +454,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1123</v>
-      </c>
-      <c r="B3">
-        <v>621</v>
+        <v>105698</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="2">
         <v>11</v>
@@ -468,13 +477,13 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5544</v>
-      </c>
-      <c r="B4">
-        <v>453</v>
+        <v>105698</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="2">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>45</v>
@@ -491,10 +500,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>9658</v>
-      </c>
-      <c r="B5">
-        <v>782</v>
+        <v>104891</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="2">
         <v>19</v>
@@ -514,10 +523,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3265</v>
-      </c>
-      <c r="B6">
-        <v>584</v>
+        <v>104891</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
       </c>
       <c r="C6" s="2">
         <v>8</v>

</xml_diff>